<commit_message>
added excel tracking file
</commit_message>
<xml_diff>
--- a/Project2/investigation.xlsx
+++ b/Project2/investigation.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="304">
   <si>
     <t>The correct answer is: 5</t>
   </si>
@@ -781,6 +783,159 @@
   </si>
   <si>
     <t>***** shapes the same Score increased******</t>
+  </si>
+  <si>
+    <t>things to do with a hashmap:</t>
+  </si>
+  <si>
+    <t>things to do with a list:</t>
+  </si>
+  <si>
+    <t>entrySet</t>
+  </si>
+  <si>
+    <t>keyset</t>
+  </si>
+  <si>
+    <t>returns</t>
+  </si>
+  <si>
+    <t>Set&lt;Entry&lt;String,String&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Set&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>things to do with a collection</t>
+  </si>
+  <si>
+    <t>Things to do with a set</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> List in Java provides ordered and indexed collection which may contain duplicates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Set provides an unordered collection of unique objects</t>
+  </si>
+  <si>
+    <t>Map provides a data structure based on key value pair and hashing</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t>LinkedHashSet</t>
+  </si>
+  <si>
+    <t>TreeSet</t>
+  </si>
+  <si>
+    <t>HashSet</t>
+  </si>
+  <si>
+    <t>Duplicate Objects</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Nulls</t>
+  </si>
+  <si>
+    <t>popular implementations</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>hashMap,
+Hashtable,
+TreeMap</t>
+  </si>
+  <si>
+    <t>HashSet,
+TreeSet,
+LinkedHashSet</t>
+  </si>
+  <si>
+    <t>ArrayList,
+LinkedList,
+Vector</t>
+  </si>
+  <si>
+    <t>not allowed</t>
+  </si>
+  <si>
+    <t>allowed</t>
+  </si>
+  <si>
+    <t>unique keys, non-unique values</t>
+  </si>
+  <si>
+    <t>maintains insertion order</t>
+  </si>
+  <si>
+    <t>unordered collection (LinkedHashSet and SortedSet maintains order)</t>
+  </si>
+  <si>
+    <t>not maintained (except in TreeMap)</t>
+  </si>
+  <si>
+    <t>just one allowed</t>
+  </si>
+  <si>
+    <t>null values, one null key. (Hashtable doesn't allow null key or values</t>
+  </si>
+  <si>
+    <t>Things to do with array</t>
+  </si>
+  <si>
+    <t>for(member:members)</t>
+  </si>
+  <si>
+    <t>for(Entry:EntrySet)</t>
+  </si>
+  <si>
+    <t>5=&gt;6</t>
+  </si>
+  <si>
+    <t>6=&gt;8</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>tf-angle=270</t>
+  </si>
+  <si>
+    <t>tf-angle=-90</t>
+  </si>
+  <si>
+    <t>tf-angle=0</t>
+  </si>
+  <si>
+    <t>tf-angle : 270 - tf-angle : -90</t>
+  </si>
+  <si>
+    <t>tf-angle : 270 - tf-angle : 0</t>
+  </si>
+  <si>
+    <t>tf-angle : 270 - tf-angle : null</t>
+  </si>
+  <si>
+    <t>tf-angle : 270 - tf-angle : 270</t>
+  </si>
+  <si>
+    <t>tf-angle=90</t>
   </si>
 </sst>
 </file>
@@ -796,18 +951,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -876,7 +1025,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -884,12 +1033,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -901,7 +1066,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5552,28 +5722,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z425"/>
+  <dimension ref="A1:AM99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M173" sqref="M173"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AK1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Y2" t="s">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AI2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AL2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5586,11 +5759,26 @@
       <c r="O3" t="s">
         <v>70</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="R3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5600,11 +5788,23 @@
       <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="R4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5614,11 +5814,23 @@
       <c r="I5" t="s">
         <v>33</v>
       </c>
-      <c r="X5" t="s">
+      <c r="R5" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -5628,11 +5840,23 @@
       <c r="I6" t="s">
         <v>32</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="R6" t="s">
+        <v>208</v>
+      </c>
+      <c r="V6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -5642,11 +5866,23 @@
       <c r="I7" t="s">
         <v>34</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="R7" t="s">
+        <v>210</v>
+      </c>
+      <c r="V7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -5656,11 +5892,23 @@
       <c r="I8" t="s">
         <v>32</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="R8" t="s">
+        <v>205</v>
+      </c>
+      <c r="V8" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>206</v>
       </c>
@@ -5670,11 +5918,23 @@
       <c r="I9" t="s">
         <v>220</v>
       </c>
-      <c r="X9" t="s">
+      <c r="R9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>294</v>
+      </c>
+      <c r="AK9" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>207</v>
       </c>
@@ -5684,11 +5944,20 @@
       <c r="I10" t="s">
         <v>221</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="R10" t="s">
+        <v>206</v>
+      </c>
+      <c r="V10" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>236</v>
+      </c>
+      <c r="AL10" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -5698,71 +5967,101 @@
       <c r="I11" t="s">
         <v>37</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="R11" t="s">
+        <v>16</v>
+      </c>
+      <c r="V11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
         <v>32</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>222</v>
       </c>
-      <c r="X13">
+      <c r="AA13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
         <v>223</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
+        <v>238</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
         <v>40</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM15" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
         <v>254</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AM16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="X17">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AK17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Y18" t="s">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AL18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z19" t="s">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM19" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z20" t="s">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM20" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -5775,11 +6074,23 @@
       <c r="O21" t="s">
         <v>249</v>
       </c>
-      <c r="X21">
+      <c r="R21" t="s">
+        <v>8</v>
+      </c>
+      <c r="V21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>251</v>
+      </c>
+      <c r="AK21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -5789,11 +6100,20 @@
       <c r="I22" t="s">
         <v>32</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="R22" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL22" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -5803,11 +6123,20 @@
       <c r="I23" t="s">
         <v>33</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="R23" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -5817,11 +6146,20 @@
       <c r="I24" t="s">
         <v>32</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="R24" t="s">
+        <v>208</v>
+      </c>
+      <c r="V24" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM24" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -5831,11 +6169,20 @@
       <c r="I25" t="s">
         <v>34</v>
       </c>
-      <c r="X25">
+      <c r="R25" t="s">
+        <v>210</v>
+      </c>
+      <c r="V25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -5845,11 +6192,20 @@
       <c r="I26" t="s">
         <v>32</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="R26" t="s">
+        <v>205</v>
+      </c>
+      <c r="V26" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>239</v>
+      </c>
+      <c r="AL26" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>206</v>
       </c>
@@ -5859,11 +6215,20 @@
       <c r="I27" t="s">
         <v>224</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="R27" t="s">
+        <v>13</v>
+      </c>
+      <c r="V27" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM27" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>207</v>
       </c>
@@ -5873,11 +6238,20 @@
       <c r="I28" t="s">
         <v>221</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="R28" t="s">
+        <v>206</v>
+      </c>
+      <c r="V28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM28" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -5887,57 +6261,78 @@
       <c r="I29" t="s">
         <v>37</v>
       </c>
-      <c r="X29">
+      <c r="R29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
         <v>32</v>
       </c>
-      <c r="X30">
+      <c r="AA30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK30">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
         <v>222</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="AA31" t="s">
+        <v>238</v>
+      </c>
+      <c r="AL31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
         <v>225</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AA32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM32" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
       <c r="I33" t="s">
         <v>32</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="AM33" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
       <c r="I34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
       <c r="I35" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>214</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -5946,113 +6341,224 @@
       <c r="O37" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="R37" t="s">
+        <v>8</v>
+      </c>
+      <c r="V37" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="R38" t="s">
+        <v>9</v>
+      </c>
+      <c r="V38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="R39" t="s">
+        <v>10</v>
+      </c>
+      <c r="V39" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>208</v>
       </c>
       <c r="I40" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="R40" t="s">
+        <v>208</v>
+      </c>
+      <c r="V40" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>210</v>
       </c>
       <c r="I41" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="R41" t="s">
+        <v>210</v>
+      </c>
+      <c r="V41" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>215</v>
       </c>
       <c r="I42" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="R42" t="s">
+        <v>205</v>
+      </c>
+      <c r="V42" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I43" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="R43" t="s">
+        <v>13</v>
+      </c>
+      <c r="V43" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I44" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="R44" t="s">
+        <v>206</v>
+      </c>
+      <c r="V44" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D45" s="1"/>
       <c r="I45" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R45" t="s">
+        <v>16</v>
+      </c>
+      <c r="V45" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="D46" s="1"/>
       <c r="I46" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="D47" s="1"/>
       <c r="I47" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="D48" s="1"/>
       <c r="I48" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="D49" s="1"/>
       <c r="I49" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA49" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="AA50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -6065,8 +6571,20 @@
       <c r="O54" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R54" t="s">
+        <v>8</v>
+      </c>
+      <c r="V54" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -6076,8 +6594,17 @@
       <c r="I55" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R55" t="s">
+        <v>9</v>
+      </c>
+      <c r="V55" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -6087,8 +6614,17 @@
       <c r="I56" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R56" t="s">
+        <v>10</v>
+      </c>
+      <c r="V56" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>204</v>
       </c>
@@ -6098,8 +6634,17 @@
       <c r="I57" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R57" t="s">
+        <v>208</v>
+      </c>
+      <c r="V57" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>205</v>
       </c>
@@ -6109,8 +6654,17 @@
       <c r="I58" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R58" t="s">
+        <v>210</v>
+      </c>
+      <c r="V58" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -6120,8 +6674,17 @@
       <c r="I59" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R59" t="s">
+        <v>205</v>
+      </c>
+      <c r="V59" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>206</v>
       </c>
@@ -6131,8 +6694,17 @@
       <c r="I60" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R60" t="s">
+        <v>13</v>
+      </c>
+      <c r="V60" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>207</v>
       </c>
@@ -6142,8 +6714,17 @@
       <c r="I61" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R61" t="s">
+        <v>206</v>
+      </c>
+      <c r="V61" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -6153,33 +6734,57 @@
       <c r="I62" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R62" t="s">
+        <v>16</v>
+      </c>
+      <c r="V62" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I63" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I64" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I65" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA65" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I66" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA66" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -6192,52 +6797,100 @@
       <c r="O71" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R71" t="s">
+        <v>8</v>
+      </c>
+      <c r="V71" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG71" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>9</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R72" t="s">
+        <v>9</v>
+      </c>
+      <c r="V72" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
       <c r="D73" t="s">
         <v>217</v>
       </c>
-      <c r="I73" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R73" t="s">
+        <v>10</v>
+      </c>
+      <c r="V73" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>204</v>
       </c>
       <c r="D74" t="s">
         <v>208</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R74" t="s">
+        <v>208</v>
+      </c>
+      <c r="V74" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>205</v>
       </c>
       <c r="D75" t="s">
         <v>210</v>
       </c>
-      <c r="I75" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R75" t="s">
+        <v>210</v>
+      </c>
+      <c r="V75" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -6247,50 +6900,89 @@
       <c r="I76" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R76" t="s">
+        <v>205</v>
+      </c>
+      <c r="V76" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>206</v>
       </c>
       <c r="D77" t="s">
         <v>16</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R77" t="s">
+        <v>13</v>
+      </c>
+      <c r="V77" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>207</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R78" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R79" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I80" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA80" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I81" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA81" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I82" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA82" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -6303,8 +6995,20 @@
       <c r="O87" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R87" t="s">
+        <v>8</v>
+      </c>
+      <c r="V87" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -6314,8 +7018,17 @@
       <c r="I88" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R88" t="s">
+        <v>9</v>
+      </c>
+      <c r="V88" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -6325,8 +7038,17 @@
       <c r="I89" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R89" t="s">
+        <v>10</v>
+      </c>
+      <c r="V89" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA89" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -6336,8 +7058,17 @@
       <c r="I90" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R90" t="s">
+        <v>208</v>
+      </c>
+      <c r="V90" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA90" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>205</v>
       </c>
@@ -6347,8 +7078,17 @@
       <c r="I91" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R91" t="s">
+        <v>210</v>
+      </c>
+      <c r="V91" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -6358,8 +7098,17 @@
       <c r="I92" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R92" t="s">
+        <v>205</v>
+      </c>
+      <c r="V92" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>206</v>
       </c>
@@ -6369,8 +7118,17 @@
       <c r="I93" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R93" t="s">
+        <v>13</v>
+      </c>
+      <c r="V93" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>207</v>
       </c>
@@ -6380,8 +7138,17 @@
       <c r="I94" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R94" t="s">
+        <v>206</v>
+      </c>
+      <c r="V94" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -6391,1549 +7158,1120 @@
       <c r="I95" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R95" t="s">
+        <v>16</v>
+      </c>
+      <c r="V95" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="I96" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="V96" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="9:27" x14ac:dyDescent="0.25">
       <c r="I97" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AA97" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="9:27" x14ac:dyDescent="0.25">
       <c r="I98" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AA98" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="99" spans="9:27" x14ac:dyDescent="0.25">
       <c r="I99" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="AA99" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" t="s">
+        <v>256</v>
+      </c>
+      <c r="L1" t="s">
+        <v>263</v>
+      </c>
+      <c r="R1" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" t="s">
+        <v>264</v>
+      </c>
+      <c r="L2" t="s">
+        <v>265</v>
+      </c>
+      <c r="R2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" t="s">
+        <v>267</v>
+      </c>
+      <c r="L3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F4" t="s">
+        <v>268</v>
+      </c>
+      <c r="L4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>266</v>
+      </c>
+      <c r="L5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+      <c r="C13" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+      <c r="C14" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E231"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>297</v>
+      </c>
+      <c r="E22" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>298</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>212</v>
+      </c>
+      <c r="E46" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>208</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>210</v>
+      </c>
+      <c r="E48" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>213</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>214</v>
+      </c>
+      <c r="E64" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>208</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>215</v>
+      </c>
+      <c r="E69" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>25</v>
+      </c>
+      <c r="E85" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>296</v>
+      </c>
+      <c r="E86" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>208</v>
+      </c>
+      <c r="E89" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>210</v>
+      </c>
+      <c r="E90" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>216</v>
+      </c>
+      <c r="E92" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>217</v>
+      </c>
+      <c r="E108" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>208</v>
+      </c>
+      <c r="E109" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>210</v>
+      </c>
+      <c r="E110" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>218</v>
+      </c>
+      <c r="E111" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+      <c r="E112" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>296</v>
+      </c>
+      <c r="E127" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>10</v>
+      </c>
+      <c r="E129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>219</v>
+      </c>
+      <c r="E130" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>208</v>
+      </c>
+      <c r="E131" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>148</v>
+      </c>
+      <c r="E132" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>210</v>
+      </c>
+      <c r="E133" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>135</v>
+      </c>
+      <c r="E134" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>13</v>
+      </c>
+      <c r="E135" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
got 2x2 prob 2
</commit_message>
<xml_diff>
--- a/Project2/investigation.xlsx
+++ b/Project2/investigation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="316">
   <si>
     <t>The correct answer is: 5</t>
   </si>
@@ -936,6 +936,42 @@
   </si>
   <si>
     <t>tf-angle=90</t>
+  </si>
+  <si>
+    <t>tf-angle : -90 - tf-angle : 270</t>
+  </si>
+  <si>
+    <t>tf-angle : -90 - tf-angle : null</t>
+  </si>
+  <si>
+    <t>tf-angle : -90 - tf-angle : 0</t>
+  </si>
+  <si>
+    <t>tf-angle : -90 - tf-angle : 90</t>
+  </si>
+  <si>
+    <t>2=&gt;5</t>
+  </si>
+  <si>
+    <t>4=&gt;3</t>
+  </si>
+  <si>
+    <t>2=&gt;8</t>
+  </si>
+  <si>
+    <t>4=&gt;8</t>
+  </si>
+  <si>
+    <t>Answer: 2</t>
+  </si>
+  <si>
+    <t>Robbie guessed: 2</t>
+  </si>
+  <si>
+    <t>hashmap.entrySet() = Entry&lt;String,String&gt;</t>
+  </si>
+  <si>
+    <t>sometimes hashmap.entrySet() = Entry&lt;String,String&gt; and sometimes Set&lt;Entry&lt;String,String&gt;&gt;?</t>
   </si>
 </sst>
 </file>
@@ -7213,7 +7249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -7292,6 +7328,16 @@
         <v>271</v>
       </c>
     </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>315</v>
+      </c>
+    </row>
     <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
@@ -7378,897 +7424,1841 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E231"/>
+  <dimension ref="A1:Y847"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>296</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="M3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>204</v>
       </c>
-      <c r="E4" t="s">
+      <c r="M4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>205</v>
       </c>
-      <c r="E5" t="s">
+      <c r="M5" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="M6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>
-      <c r="E7" t="s">
+      <c r="M7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>207</v>
       </c>
-      <c r="E8" t="s">
+      <c r="M8" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="M9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Y9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>297</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>299</v>
+      </c>
+      <c r="L22" t="str">
+        <f>Y2</f>
+        <v>1=&gt;4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>296</v>
+      </c>
+      <c r="P22" t="s">
+        <v>297</v>
+      </c>
+      <c r="S22" t="s">
+        <v>304</v>
+      </c>
+      <c r="X22" t="str">
+        <f>Y10</f>
+        <v>1=&gt;3</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" t="s">
+        <v>10</v>
+      </c>
+      <c r="P24" t="s">
+        <v>10</v>
+      </c>
+      <c r="S24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>208</v>
       </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" t="s">
+        <v>204</v>
+      </c>
+      <c r="P25" t="s">
+        <v>208</v>
+      </c>
+      <c r="S25" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>209</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
+        <v>205</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>210</v>
+      </c>
+      <c r="S26" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>210</v>
       </c>
-      <c r="E27" t="s">
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>220</v>
+      </c>
+      <c r="M27" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>205</v>
+      </c>
+      <c r="S27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>211</v>
       </c>
-      <c r="E28" t="s">
+      <c r="D28" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" t="s">
+        <v>221</v>
+      </c>
+      <c r="M28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>13</v>
+      </c>
+      <c r="S28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="E29" t="s">
+      <c r="D29" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M29" t="s">
+        <v>207</v>
+      </c>
+      <c r="P29" t="s">
+        <v>206</v>
+      </c>
+      <c r="S29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
-      <c r="E30" t="s">
+      <c r="D30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M30" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" t="s">
+        <v>16</v>
+      </c>
+      <c r="S30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>222</v>
+      </c>
+      <c r="S31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>223</v>
+      </c>
+      <c r="S32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>40</v>
+      </c>
+      <c r="S33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>298</v>
       </c>
-      <c r="E43" t="s">
+      <c r="D43" t="s">
+        <v>296</v>
+      </c>
+      <c r="G43" t="s">
+        <v>300</v>
+      </c>
+      <c r="L43" t="str">
+        <f>Y3</f>
+        <v>2=&gt;5</v>
+      </c>
+      <c r="M43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>297</v>
+      </c>
+      <c r="S43" t="s">
+        <v>305</v>
+      </c>
+      <c r="X43" t="str">
+        <f>Y11</f>
+        <v>2=&gt;3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
-      <c r="E44" t="s">
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M44" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>9</v>
+      </c>
+      <c r="S44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
-      <c r="E45" t="s">
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M45" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P45" t="s">
+        <v>10</v>
+      </c>
+      <c r="S45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>212</v>
       </c>
-      <c r="E46" t="s">
+      <c r="D46" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>34</v>
+      </c>
+      <c r="M46" t="s">
+        <v>204</v>
+      </c>
+      <c r="P46" t="s">
+        <v>208</v>
+      </c>
+      <c r="S46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>208</v>
       </c>
-      <c r="E47" t="s">
+      <c r="D47" t="s">
+        <v>205</v>
+      </c>
+      <c r="G47" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>210</v>
+      </c>
+      <c r="S47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>210</v>
       </c>
-      <c r="E48" t="s">
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" t="s">
+        <v>224</v>
+      </c>
+      <c r="M48" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P48" t="s">
+        <v>205</v>
+      </c>
+      <c r="S48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
-      <c r="E49" t="s">
+      <c r="D49" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" t="s">
+        <v>221</v>
+      </c>
+      <c r="M49" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P49" t="s">
+        <v>13</v>
+      </c>
+      <c r="S49" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>213</v>
       </c>
-      <c r="E50" t="s">
+      <c r="D50" t="s">
+        <v>207</v>
+      </c>
+      <c r="G50" t="s">
+        <v>37</v>
+      </c>
+      <c r="M50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P50" t="s">
+        <v>206</v>
+      </c>
+      <c r="S50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>32</v>
+      </c>
+      <c r="P51" t="s">
+        <v>16</v>
+      </c>
+      <c r="S51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>222</v>
+      </c>
+      <c r="S52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>225</v>
+      </c>
+      <c r="S53" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>32</v>
+      </c>
+      <c r="S54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>214</v>
       </c>
-      <c r="E64" t="s">
+      <c r="D64" t="s">
+        <v>296</v>
+      </c>
+      <c r="G64" t="s">
+        <v>301</v>
+      </c>
+      <c r="L64" t="str">
+        <f>Y4</f>
+        <v>3=&gt;4</v>
+      </c>
+      <c r="M64" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>297</v>
+      </c>
+      <c r="S64" t="s">
+        <v>306</v>
+      </c>
+      <c r="X64" t="str">
+        <f>Y12</f>
+        <v>3=&gt;4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>9</v>
       </c>
-      <c r="E65" t="s">
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" t="s">
+        <v>33</v>
+      </c>
+      <c r="M65" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>9</v>
+      </c>
+      <c r="S65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>10</v>
       </c>
-      <c r="E66" t="s">
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" t="s">
+        <v>32</v>
+      </c>
+      <c r="M66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P66" t="s">
+        <v>10</v>
+      </c>
+      <c r="S66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>208</v>
       </c>
-      <c r="E67" t="s">
+      <c r="D67" t="s">
+        <v>204</v>
+      </c>
+      <c r="G67" t="s">
+        <v>34</v>
+      </c>
+      <c r="M67" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P67" t="s">
+        <v>208</v>
+      </c>
+      <c r="S67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>210</v>
       </c>
-      <c r="E68" t="s">
+      <c r="D68" t="s">
+        <v>205</v>
+      </c>
+      <c r="G68" t="s">
+        <v>32</v>
+      </c>
+      <c r="M68" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P68" t="s">
+        <v>210</v>
+      </c>
+      <c r="S68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>215</v>
       </c>
-      <c r="E69" t="s">
+      <c r="D69" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" t="s">
+        <v>226</v>
+      </c>
+      <c r="M69" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P69" t="s">
+        <v>205</v>
+      </c>
+      <c r="S69" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
-      <c r="E70" t="s">
+      <c r="D70" t="s">
+        <v>206</v>
+      </c>
+      <c r="G70" t="s">
+        <v>221</v>
+      </c>
+      <c r="M70" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P70" t="s">
+        <v>13</v>
+      </c>
+      <c r="S70" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
-      <c r="E71" t="s">
+      <c r="D71" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+      <c r="G71" t="s">
+        <v>37</v>
+      </c>
+      <c r="M71" t="s">
+        <v>207</v>
+      </c>
+      <c r="P71" t="s">
+        <v>206</v>
+      </c>
+      <c r="S71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="G72" t="s">
+        <v>32</v>
+      </c>
+      <c r="M72" t="s">
+        <v>16</v>
+      </c>
+      <c r="P72" t="s">
+        <v>16</v>
+      </c>
+      <c r="S72" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>222</v>
+      </c>
+      <c r="S73" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>227</v>
+      </c>
+      <c r="S74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>40</v>
+      </c>
+      <c r="S75" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>254</v>
+      </c>
+      <c r="S76" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E85" t="s">
+      <c r="D85" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="L85" s="10" t="str">
+        <f>Y5</f>
+        <v>4=&gt;5</v>
+      </c>
+      <c r="M85" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P85" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="S85" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="X85" s="10" t="str">
+        <f>Y13</f>
+        <v>4=&gt;3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>296</v>
       </c>
-      <c r="E86" t="s">
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86" t="s">
+        <v>32</v>
+      </c>
+      <c r="M86" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P86" t="s">
+        <v>9</v>
+      </c>
+      <c r="S86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
-      <c r="E87" t="s">
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" t="s">
+        <v>33</v>
+      </c>
+      <c r="M87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P87" t="s">
+        <v>10</v>
+      </c>
+      <c r="S87" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>10</v>
       </c>
-      <c r="E88" t="s">
+      <c r="D88" t="s">
+        <v>204</v>
+      </c>
+      <c r="G88" t="s">
+        <v>32</v>
+      </c>
+      <c r="M88" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P88" t="s">
+        <v>208</v>
+      </c>
+      <c r="S88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>208</v>
       </c>
-      <c r="E89" t="s">
+      <c r="D89" t="s">
+        <v>205</v>
+      </c>
+      <c r="G89" t="s">
+        <v>34</v>
+      </c>
+      <c r="M89" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P89" t="s">
+        <v>210</v>
+      </c>
+      <c r="S89" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>210</v>
       </c>
-      <c r="E90" t="s">
+      <c r="D90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>32</v>
+      </c>
+      <c r="M90" t="s">
+        <v>13</v>
+      </c>
+      <c r="P90" t="s">
+        <v>205</v>
+      </c>
+      <c r="S90" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
-      <c r="E91" t="s">
+      <c r="D91" t="s">
+        <v>206</v>
+      </c>
+      <c r="G91" t="s">
+        <v>228</v>
+      </c>
+      <c r="M91" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P91" t="s">
+        <v>13</v>
+      </c>
+      <c r="S91" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>216</v>
       </c>
-      <c r="E92" t="s">
+      <c r="D92" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>221</v>
+      </c>
+      <c r="M92" t="s">
+        <v>207</v>
+      </c>
+      <c r="P92" t="s">
+        <v>206</v>
+      </c>
+      <c r="S92" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
-      <c r="E93" t="s">
+      <c r="D93" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>37</v>
+      </c>
+      <c r="M93" t="s">
+        <v>16</v>
+      </c>
+      <c r="P93" t="s">
+        <v>16</v>
+      </c>
+      <c r="S93" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>32</v>
+      </c>
+      <c r="S94" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>222</v>
+      </c>
+      <c r="S95" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>229</v>
+      </c>
+      <c r="S96" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>9</v>
       </c>
-      <c r="E106" t="s">
+      <c r="D106" t="s">
+        <v>296</v>
+      </c>
+      <c r="G106" t="s">
+        <v>301</v>
+      </c>
+      <c r="L106" t="str">
+        <f>Y6</f>
+        <v>5=&gt;3</v>
+      </c>
+      <c r="M106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P106" t="s">
+        <v>297</v>
+      </c>
+      <c r="S106" t="s">
+        <v>305</v>
+      </c>
+      <c r="X106" t="str">
+        <f>Y14</f>
+        <v>5=&gt;3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>10</v>
       </c>
-      <c r="E107" t="s">
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+      <c r="G107" t="s">
+        <v>33</v>
+      </c>
+      <c r="M107" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P107" t="s">
+        <v>9</v>
+      </c>
+      <c r="S107" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>217</v>
       </c>
-      <c r="E108" t="s">
+      <c r="D108" t="s">
+        <v>10</v>
+      </c>
+      <c r="G108" t="s">
+        <v>32</v>
+      </c>
+      <c r="M108" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P108" t="s">
+        <v>10</v>
+      </c>
+      <c r="S108" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>208</v>
       </c>
-      <c r="E109" t="s">
+      <c r="D109" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>34</v>
+      </c>
+      <c r="M109" t="s">
+        <v>204</v>
+      </c>
+      <c r="P109" t="s">
+        <v>208</v>
+      </c>
+      <c r="S109" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>210</v>
       </c>
-      <c r="E110" t="s">
+      <c r="D110" t="s">
+        <v>205</v>
+      </c>
+      <c r="G110" t="s">
+        <v>32</v>
+      </c>
+      <c r="M110" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P110" t="s">
+        <v>210</v>
+      </c>
+      <c r="S110" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>218</v>
       </c>
-      <c r="E111" t="s">
+      <c r="D111" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111" t="s">
+        <v>230</v>
+      </c>
+      <c r="M111" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P111" t="s">
+        <v>205</v>
+      </c>
+      <c r="S111" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>16</v>
       </c>
-      <c r="E112" t="s">
+      <c r="D112" t="s">
+        <v>206</v>
+      </c>
+      <c r="G112" t="s">
+        <v>221</v>
+      </c>
+      <c r="M112" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P112" t="s">
+        <v>13</v>
+      </c>
+      <c r="S112" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>207</v>
+      </c>
+      <c r="G113" t="s">
+        <v>231</v>
+      </c>
+      <c r="P113" t="s">
+        <v>206</v>
+      </c>
+      <c r="S113" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" t="s">
+        <v>222</v>
+      </c>
+      <c r="P114" t="s">
+        <v>16</v>
+      </c>
+      <c r="S114" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>232</v>
+      </c>
+      <c r="S115" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>40</v>
+      </c>
+      <c r="S116" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G117" t="s">
+        <v>253</v>
+      </c>
+      <c r="S117" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>296</v>
       </c>
-      <c r="E127" t="s">
+      <c r="D127" t="s">
+        <v>296</v>
+      </c>
+      <c r="G127" t="s">
+        <v>302</v>
+      </c>
+      <c r="L127" t="str">
+        <f>Y7</f>
+        <v>6=&gt;4</v>
+      </c>
+      <c r="M127" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P127" t="s">
+        <v>297</v>
+      </c>
+      <c r="S127" t="s">
+        <v>307</v>
+      </c>
+      <c r="X127" t="str">
+        <f>Y15</f>
+        <v>6=&gt;3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>9</v>
       </c>
-      <c r="E128" t="s">
+      <c r="D128" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G128" t="s">
+        <v>32</v>
+      </c>
+      <c r="M128" t="s">
+        <v>9</v>
+      </c>
+      <c r="P128" t="s">
+        <v>9</v>
+      </c>
+      <c r="S128" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>10</v>
       </c>
-      <c r="E129" t="s">
+      <c r="D129" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G129" t="s">
+        <v>33</v>
+      </c>
+      <c r="M129" t="s">
+        <v>10</v>
+      </c>
+      <c r="P129" t="s">
+        <v>10</v>
+      </c>
+      <c r="S129" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>219</v>
       </c>
-      <c r="E130" t="s">
+      <c r="D130" t="s">
+        <v>204</v>
+      </c>
+      <c r="G130" t="s">
+        <v>32</v>
+      </c>
+      <c r="M130" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P130" t="s">
+        <v>208</v>
+      </c>
+      <c r="S130" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>208</v>
       </c>
-      <c r="E131" t="s">
+      <c r="D131" t="s">
+        <v>205</v>
+      </c>
+      <c r="G131" t="s">
+        <v>34</v>
+      </c>
+      <c r="M131" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P131" t="s">
+        <v>210</v>
+      </c>
+      <c r="S131" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>148</v>
       </c>
-      <c r="E132" t="s">
+      <c r="D132" t="s">
+        <v>13</v>
+      </c>
+      <c r="G132" t="s">
+        <v>32</v>
+      </c>
+      <c r="M132" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P132" t="s">
+        <v>205</v>
+      </c>
+      <c r="S132" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>210</v>
       </c>
-      <c r="E133" t="s">
+      <c r="D133" t="s">
+        <v>206</v>
+      </c>
+      <c r="G133" t="s">
+        <v>233</v>
+      </c>
+      <c r="M133" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P133" t="s">
+        <v>13</v>
+      </c>
+      <c r="S133" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>135</v>
       </c>
-      <c r="E134" t="s">
+      <c r="D134" t="s">
+        <v>207</v>
+      </c>
+      <c r="G134" t="s">
+        <v>221</v>
+      </c>
+      <c r="M134" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P134" t="s">
+        <v>206</v>
+      </c>
+      <c r="S134" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>13</v>
       </c>
-      <c r="E135" t="s">
+      <c r="D135" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" t="s">
+        <v>37</v>
+      </c>
+      <c r="M135" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P135" t="s">
+        <v>16</v>
+      </c>
+      <c r="S135" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>16</v>
       </c>
-      <c r="E136" t="s">
+      <c r="G136" t="s">
+        <v>32</v>
+      </c>
+      <c r="M136" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="S136" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G137" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="S137" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G138" t="s">
+        <v>234</v>
+      </c>
+      <c r="S138" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G139" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>40</v>
+    <row r="728" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A728" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="730" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A730" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A731" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="733" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A733" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="735" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A735" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A736" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="738" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A738" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="740" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="741" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="745" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="746" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="748" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="750" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="751" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="753" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="755" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="756" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="758" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A758" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="760" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A760" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A763" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="765" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A765" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="766" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A766" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="768" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A768" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="770" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A770" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A771" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A773" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A775" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A778" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A780" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A781" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A783" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A785" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A786" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A788" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A790" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A791" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A793" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A795" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A796" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A798" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A800" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A801" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A803" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A805" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A806" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A808" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A810" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A811" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A813" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A815" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="818" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="820" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="821" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="823" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A823" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="825" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A825" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="826" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A826" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="828" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A828" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="830" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A830" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="831" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A831" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="833" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A833" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="835" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A835" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="836" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A836" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="838" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A838" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="840" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A840" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="841" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A841" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="843" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A843" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="845" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A845" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="846" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A846" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="847" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A847" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>